<commit_message>
Updated Plan Updated Syllabus Updated with Lecture 6
</commit_message>
<xml_diff>
--- a/plan-AD18.xlsx
+++ b/plan-AD18.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\tc2020\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5042D07-04B2-495B-BC98-7833F4A8CA59}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="17100" windowHeight="6540"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="17100" windowHeight="6540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
   <si>
     <t>Fecha</t>
   </si>
@@ -79,9 +85,6 @@
   </si>
   <si>
     <t>Repaso</t>
-  </si>
-  <si>
-    <t>Medio Término</t>
   </si>
   <si>
     <t>Derivación GLC</t>
@@ -192,14 +195,28 @@
   </si>
   <si>
     <t>29_LimitesMT</t>
+  </si>
+  <si>
+    <t>Examen 1</t>
+  </si>
+  <si>
+    <t>Examen 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -227,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -241,21 +258,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
-    <dxf>
-      <numFmt numFmtId="21" formatCode="dd\-mmm"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -266,7 +279,17 @@
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="dd\-mmm"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -274,19 +297,22 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E31" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
-  <autoFilter ref="A1:E31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E31" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E31" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Fecha" dataDxfId="0"/>
-    <tableColumn id="2" name="Temas" dataDxfId="1"/>
-    <tableColumn id="3" name="Slides" dataDxfId="6"/>
-    <tableColumn id="4" name="Tarea" dataDxfId="5"/>
-    <tableColumn id="5" name="Se entrega" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Fecha" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Temas" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Slides" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Tarea" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Se entrega" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -335,7 +361,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -368,9 +394,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -403,6 +446,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -578,11 +638,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +680,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -631,10 +691,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="2">
         <v>43329</v>
@@ -648,13 +708,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="2">
-        <v>43332</v>
+        <v>43336</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -665,7 +725,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -677,7 +737,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -689,13 +749,13 @@
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="2">
-        <v>43342</v>
+        <v>43343</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -706,7 +766,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -718,7 +778,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -730,7 +790,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -742,24 +802,21 @@
         <v>12</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="2">
-        <v>43356</v>
+        <v>43363</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>43353</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>45</v>
+      <c r="B12" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -770,6 +827,9 @@
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="C13" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="D13" s="3" t="s">
         <v>13</v>
       </c>
@@ -785,7 +845,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -797,10 +857,10 @@
         <v>16</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" s="2">
         <v>43388</v>
@@ -819,6 +879,9 @@
       <c r="A17" s="2">
         <v>43370</v>
       </c>
+      <c r="B17" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -829,7 +892,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="1"/>
     </row>
@@ -841,7 +904,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="1"/>
     </row>
@@ -859,7 +922,10 @@
         <v>43384</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="E21" s="1"/>
     </row>
@@ -868,40 +934,35 @@
         <v>43388</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>43391</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="D23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="5">
+        <v>43405</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>43395</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="2">
-        <v>43405</v>
+      <c r="B24" s="6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -909,72 +970,67 @@
         <v>43398</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="1"/>
+        <v>52</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>43402</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" s="1"/>
+        <v>53</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>43405</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E27" s="1"/>
+        <v>53</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>43409</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E28" s="1"/>
+        <v>54</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>43412</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E29" s="1"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>43416</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E30" s="2">
+        <v>34</v>
+      </c>
+      <c r="E30" s="5">
         <v>43419</v>
       </c>
     </row>
@@ -983,15 +1039,15 @@
         <v>43419</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E31" s="2">
+        <v>36</v>
+      </c>
+      <c r="E31" s="5">
         <v>43425</v>
       </c>
     </row>
@@ -1006,7 +1062,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1018,7 +1074,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>